<commit_message>
Updated version to 2.5.0
</commit_message>
<xml_diff>
--- a/documents/Published/Text Wrapper/TextWrapperByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Text Wrapper/TextWrapperByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-kajoll.FAREAST\Desktop\text wrapper smaan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAQCustomVisual\documents\Published\Text Wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42112102-53E9-4B06-9818-C6A71AA0C857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" xr2:uid="{CFA628E8-139E-4A70-BE7A-AA996D28E374}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFA628E8-139E-4A70-BE7A-AA996D28E374}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>S no</t>
   </si>
@@ -191,63 +192,120 @@
     <t>Text settings</t>
   </si>
   <si>
-    <t>Update text color, text size and text to append</t>
+    <t>Display text string</t>
+  </si>
+  <si>
+    <t>Check out for numeric value</t>
+  </si>
+  <si>
+    <t>Check output for text value</t>
+  </si>
+  <si>
+    <t>Numeric value should be displayed</t>
+  </si>
+  <si>
+    <t>1. Drag 'Values' column from 'Measure data' table into 'Field' field</t>
+  </si>
+  <si>
+    <t>What is your salary range?' text should be displayed in the visual</t>
+  </si>
+  <si>
+    <t>1. Drag 'Column1' column from 'Column data' table into 'Field' field of text wrapper visual
+2. Select slicer visual from 'Visualizations' pane. Drag 'Column1' column from 'Column data' table into 'Field' field
+3. Click on 'What is your salary range?' checkbox</t>
+  </si>
+  <si>
+    <t>1. Drag 'Column1' column from 'Column data' table into 'Field' field of text wrapper visual
+2. Select slicer visual from 'Visualizations' pane. Drag 'Column1' column from 'Column data' table into 'Field' field</t>
+  </si>
+  <si>
+    <t>1. Drag 'Column1' column from 'Column data' table into 'Field' field of text wrapper visual
+2. Select slicer visual from 'Visualizations' pane. Drag 'Column1' column from 'Column data' table into 'Field' field
+3. Click on 'What is your salary range?' checkbox and 'What is your job title' checkbox</t>
+  </si>
+  <si>
+    <t>Display error message part 1</t>
+  </si>
+  <si>
+    <t>Display error message part 2</t>
+  </si>
+  <si>
+    <t>"Query returned more than one row, please filter data to return one row" text should be displayed in the visual</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Static Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Features for static text </t>
+  </si>
+  <si>
+    <t>1. Check Font style
+2. Check Font Family
+3. Check Text Highlighter
+4. Check Colon
+5. Check Position of the static text(Text Position)- suffix or prefix</t>
+  </si>
+  <si>
+    <t>Dynamic Text</t>
+  </si>
+  <si>
+    <t>User will drag the column to the Field</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>toggle option is there</t>
+  </si>
+  <si>
+    <t>Colon appears with the appearance of static text and then you can remove the colon with the toggle button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colon will appear or disappear in the presence of static text </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check Font style 
+2. Check Font Family
+3. Check Text Highlighter
+</t>
+  </si>
+  <si>
+    <t>1. Bold, Italics and Underline are by default off.
+2. Segoe UI Semibold is the default font family.
+3. Text highlighter default value is set to white.</t>
+  </si>
+  <si>
+    <t>Update text color, text size</t>
+  </si>
+  <si>
+    <t>1. Bold, Italics and Underline are by default off.
+2. Colon will be set to 'off' by default. Segoe UI Semibold is the default font family.
+3. Text Position will be set to suffix by default. Text highlighter default value is set to white. Add any text to "Text to append" field say 'Hello world', the text 'Hello world' will be appended as suffix with a colon by default.</t>
   </si>
   <si>
     <t>1. Go to formatting pane
 2. Go to 'Text settings' option
 3. Update color to 'blue' 
-4. Update text size to '25'
-5. Update text to append to 'Hello world'</t>
-  </si>
-  <si>
-    <t>Display text string</t>
-  </si>
-  <si>
-    <t>Check out for numeric value</t>
-  </si>
-  <si>
-    <t>Check output for text value</t>
-  </si>
-  <si>
-    <t>Numeric value should be displayed</t>
-  </si>
-  <si>
-    <t>1. Drag 'Values' column from 'Measure data' table into 'Field' field</t>
-  </si>
-  <si>
-    <t>What is your salary range?' text should be displayed in the visual</t>
-  </si>
-  <si>
-    <t>1. Drag 'Column1' column from 'Column data' table into 'Field' field of text wrapper visual
-2. Select slicer visual from 'Visualizations' pane. Drag 'Column1' column from 'Column data' table into 'Field' field
-3. Click on 'What is your salary range?' checkbox</t>
-  </si>
-  <si>
-    <t>1. Drag 'Column1' column from 'Column data' table into 'Field' field of text wrapper visual
-2. Select slicer visual from 'Visualizations' pane. Drag 'Column1' column from 'Column data' table into 'Field' field</t>
-  </si>
-  <si>
-    <t>1. Drag 'Column1' column from 'Column data' table into 'Field' field of text wrapper visual
-2. Select slicer visual from 'Visualizations' pane. Drag 'Column1' column from 'Column data' table into 'Field' field
-3. Click on 'What is your salary range?' checkbox and 'What is your job title' checkbox</t>
-  </si>
-  <si>
-    <t>Display error message part 1</t>
-  </si>
-  <si>
-    <t>Display error message part 2</t>
-  </si>
-  <si>
-    <t>"Query returned more than one row, please filter data to return one row" text should be displayed in the visual</t>
-  </si>
-  <si>
-    <t>NA</t>
+4. Update text size to '25'</t>
   </si>
   <si>
     <t>1. Text color will be set to 'blue'
-2. Text size will be set to 25 pt.
-3. 'Hello world' text will be appended to text string</t>
+2. Text size will be set to 25 pt.</t>
+  </si>
+  <si>
+    <t>Internet Explorer</t>
+  </si>
+  <si>
+    <t>Power BI Desktop</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -364,14 +422,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,7 +455,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -420,6 +473,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,6 +506,1419 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3410378</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2734021</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D83AC67E-FE76-4CFF-984A-6347EF3CBD7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15525750" y="447675"/>
+          <a:ext cx="3067478" cy="2476846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3238924</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2553006</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3692B31-E080-4C17-AA14-CD68AEAE2D9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19088100" y="552450"/>
+          <a:ext cx="3038899" cy="2191056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3581852</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2429169</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0385F18F-7BD4-46C3-A409-2737F08A0EBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22526625" y="514350"/>
+          <a:ext cx="3238952" cy="2105319"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>428625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3229399</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2076680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1797378B-2636-47FE-8644-C933ECC9ECE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26098500" y="619125"/>
+          <a:ext cx="3038899" cy="1648055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5127472</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2047875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB24C489-13FE-4175-8499-C7584F74EBEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15306675" y="3705225"/>
+          <a:ext cx="5003647" cy="1762125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47676</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>400051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4594773</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2152651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD0682BB-0559-4499-8049-5A6DCBEA6DB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20688351" y="3819526"/>
+          <a:ext cx="4547097" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4917499</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2057750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A4D2E0F-2F0E-40CF-810B-A4FF0E5B2406}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25412700" y="3819525"/>
+          <a:ext cx="4765099" cy="1657700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>533400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4099482</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1895722</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B7E19F0-D62C-4043-8600-2BF18DDFA44B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30441900" y="3952875"/>
+          <a:ext cx="3918507" cy="1362322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5391856</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2076720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC791A6-57DE-483A-A2CF-7295648F2F42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15516225" y="6115050"/>
+          <a:ext cx="5058481" cy="1933845"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>285751</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4532904</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1695451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{474C0688-3EFD-456C-B318-62073B8B8380}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20669251" y="6257926"/>
+          <a:ext cx="4504328" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4829175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1990725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04BB1E73-E660-46DE-AEE1-464D8738F867}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25536525" y="6134100"/>
+          <a:ext cx="4552950" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4048125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1924296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A599025D-BB33-4388-A911-FE51646AB188}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30346650" y="6134100"/>
+          <a:ext cx="3962400" cy="1762371"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5248276</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2086500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4532B989-65BD-4D12-BEE1-97DF9DBC25F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15497176" y="8467725"/>
+          <a:ext cx="4933950" cy="1857900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4536863</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1952625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8253390-9DFC-4E8A-B9CF-5D7F6B81CA4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20774026" y="8401050"/>
+          <a:ext cx="4403512" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4810125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1981441</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E05DE263-5B4F-45F4-9D3F-7C825578685B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25555575" y="8496300"/>
+          <a:ext cx="4514850" cy="1724266"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4019551</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1872168</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B327804-DF8A-40B0-B5CF-4F94571DB390}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30508576" y="8696325"/>
+          <a:ext cx="3771900" cy="1414968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4391524</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2295821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA2E0D8F-E211-491A-94F8-124F6EB1C6A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16002000" y="10858500"/>
+          <a:ext cx="3572374" cy="2124371"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3600878</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1990968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{741B1BC7-1673-4BFE-A738-15836B698457}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21174075" y="10934700"/>
+          <a:ext cx="3067478" cy="1743318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4048125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2193925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E003FF0-A284-49A1-81B9-4AE8E79273BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26165175" y="10944225"/>
+          <a:ext cx="3143250" cy="1936750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3667552</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2410132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BA82332-061E-474F-81B5-5114C0A2B1FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30870525" y="10896600"/>
+          <a:ext cx="3057952" cy="2200582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5039342</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1933788</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B447087-72C9-499E-BA85-9CA6CAF79D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15801975" y="13801725"/>
+          <a:ext cx="4420217" cy="1524213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>819151</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>94806</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4133850</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3286125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19584007-8651-42DA-A053-1C0A39959989}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21459826" y="13486956"/>
+          <a:ext cx="3314699" cy="3191319"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>406142</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4852147</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2516131</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB49999-64EE-44DD-BDF0-D8651098F3B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25302883" y="13785966"/>
+          <a:ext cx="4784911" cy="2109989"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4022912</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2812003</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59CAFC03-2AB5-4DDA-AB3B-558330A263E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30547236" y="13570324"/>
+          <a:ext cx="3709147" cy="2621503"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1703294</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3322770</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3843617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06E54ED7-DDD6-4D1B-935F-87C13988076B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16864853" y="16864852"/>
+          <a:ext cx="1619476" cy="3697941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1344706</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>201708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2983235</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3664326</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8583D051-F0E9-4C19-825F-C6F0A460D7FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21963530" y="16920884"/>
+          <a:ext cx="1638529" cy="3462618"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3181581</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3810000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E1BDD1C-F460-447E-A346-532894459D28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26759647" y="16842441"/>
+          <a:ext cx="1657581" cy="3686735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1075765</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>212912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2752399</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3720353</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E69187D4-F682-4F4D-A23B-D1B28EEBA1AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31309236" y="16932088"/>
+          <a:ext cx="1676634" cy="3507441"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5395786</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3208115</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A7B3EDC-AAEF-4AE5-99BF-2AE24974C33A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15441706" y="20742087"/>
+          <a:ext cx="5115639" cy="3096057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>324971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4974425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2697027</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B071AD4-2047-4F87-B649-ECA74580FB1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20630031" y="20955000"/>
+          <a:ext cx="4963218" cy="2372056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>257736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4986618</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2820319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56A32C5E-1BC2-4432-B10E-A2303E7332F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25717500" y="20887765"/>
+          <a:ext cx="4896971" cy="2562583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>358587</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>201705</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4605618</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2707130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FF462DF-BF2E-4677-8D66-1F95B10A30A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30984263" y="20831734"/>
+          <a:ext cx="4247031" cy="2505425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -734,10 +2218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C560CE-405B-4CA8-AB3A-A0EEBCD256B2}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,129 +2229,186 @@
     <col min="2" max="2" width="28.140625" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="48.140625" customWidth="1"/>
-    <col min="5" max="5" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="99.5703125" customWidth="1"/>
+    <col min="6" max="6" width="81.85546875" customWidth="1"/>
+    <col min="7" max="7" width="75.140625" customWidth="1"/>
+    <col min="8" max="8" width="75" customWidth="1"/>
+    <col min="9" max="9" width="71.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="F1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="201" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="4" t="s">
+    <row r="4" spans="1:9" ht="178.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="E5" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="3" t="s">
+    </row>
+    <row r="6" spans="1:9" ht="213" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>2</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="263.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>3</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="C7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="307.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>4</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="260.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>5</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -875,6 +2416,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -882,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BDF48F-142E-4DA3-AA46-5DE95B2DDBCD}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,274 +2434,274 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>49</v>
+      <c r="C6" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>49</v>
+      <c r="C14" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="19"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="A21" s="12">
         <v>18</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="12" t="s">
+      <c r="A22" s="13"/>
+      <c r="B22" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="19"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="19"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="20"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>19</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
+      <c r="A27" s="4">
         <v>20</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>49</v>
+      <c r="C27" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>